<commit_message>
Work in progress: GUI
</commit_message>
<xml_diff>
--- a/src_python/rs485_pump_test/gui.xlsx
+++ b/src_python/rs485_pump_test/gui.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\project-TWT-jetting-grid\src_python\rs485_pump_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5934C0FC-5E6F-42F1-AC1B-622403B07222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9340917B-8889-4C62-87EB-67B75FAF76F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="18648" windowHeight="14100" xr2:uid="{0E668B54-C984-4221-A3D2-B61E66A1B4EA}"/>
+    <workbookView xWindow="1418" yWindow="780" windowWidth="18967" windowHeight="14392" xr2:uid="{0E668B54-C984-4221-A3D2-B61E66A1B4EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Start/stop</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>#11 overcurrent</t>
   </si>
   <si>
@@ -131,20 +128,35 @@
     <t>O</t>
   </si>
   <si>
-    <t>Limits:</t>
-  </si>
-  <si>
     <t>20 - 50</t>
   </si>
   <si>
     <t>% FS</t>
+  </si>
+  <si>
+    <t>0 - 5</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Limits</t>
+  </si>
+  <si>
+    <t>Error status</t>
+  </si>
+  <si>
+    <t>No errors</t>
+  </si>
+  <si>
+    <t>Possible errors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +164,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -169,13 +203,181 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,193 +692,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B66F21C-9B50-4C31-9F38-AD747A968C73}">
-  <dimension ref="B3:K16"/>
+  <dimension ref="B2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" customWidth="1"/>
-    <col min="9" max="9" width="8.21875" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="1.33203125" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" customWidth="1"/>
+    <col min="7" max="7" width="3.53125" customWidth="1"/>
+    <col min="8" max="8" width="1.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.19921875" customWidth="1"/>
+    <col min="12" max="12" width="1.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
+      <c r="N2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B4" s="12"/>
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J4" s="25">
+        <v>50</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="N4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="25">
+        <v>2</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="11"/>
+      <c r="N5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="25">
+        <v>25</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B7" s="12"/>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="25">
+        <v>310</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="N7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B8" s="12"/>
+      <c r="C8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>50</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="H10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="N10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B11" s="12"/>
+      <c r="C11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="N11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B12" s="12"/>
+      <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="11"/>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B13" s="12"/>
+      <c r="C13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="N13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="N14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="11"/>
+      <c r="N15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B16" s="12"/>
+      <c r="C16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="23">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="E16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="12"/>
+      <c r="C17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="23">
+        <v>20</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="12"/>
+      <c r="C18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8">
-        <v>310</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="E18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>2.5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K16" t="s">
-        <v>13</v>
-      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>